<commit_message>
Uodated the clean data
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Java\OnlineModelLearning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Python\CS467\SentimentSocialNets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="358">
   <si>
     <t>c_emo</t>
   </si>
@@ -1029,12 +1029,84 @@
   </si>
   <si>
     <t>budlightliving,budlightsensation</t>
+  </si>
+  <si>
+    <t>Twitter Followers</t>
+  </si>
+  <si>
+    <t>Twitter Following</t>
+  </si>
+  <si>
+    <t>Twitter Reply Count</t>
+  </si>
+  <si>
+    <t>Twitter Reply to</t>
+  </si>
+  <si>
+    <t>Twitter Retweet of</t>
+  </si>
+  <si>
+    <t>Twitter Retweets</t>
+  </si>
+  <si>
+    <t>Twitter Tweets</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>http://twitter.com/BudLightCA/statuses/466603056201998336</t>
+  </si>
+  <si>
+    <t>http://twitter.com/CLAWCKR/statuses/466259503177277441</t>
+  </si>
+  <si>
+    <t>http://twitter.com/BudLightCA/statuses/466766799951122433</t>
+  </si>
+  <si>
+    <t>http://twitter.com/BudLightCA/statuses/466941611415728128</t>
+  </si>
+  <si>
+    <t>http://twitter.com/BudLightCA/statuses/467017888571068418</t>
+  </si>
+  <si>
+    <t>http://twitter.com/ConstanceChan/statuses/467081075068784640</t>
+  </si>
+  <si>
+    <t>http://twitter.com/BudLightCA/statuses/467084361687633920</t>
+  </si>
+  <si>
+    <t>http://twitter.com/cbwcbwcbw/statuses/467164972934365184</t>
+  </si>
+  <si>
+    <t>http://twitter.com/BudLightCA/statuses/467411575570464768</t>
+  </si>
+  <si>
+    <t>http://twitter.com/MarcLombo/statuses/467423297266016257</t>
+  </si>
+  <si>
+    <t>http://twitter.com/ryan_maccarthy/statuses/467448776076951552</t>
+  </si>
+  <si>
+    <t>http://twitter.com/Vallisofneptune/statuses/467381852492140544</t>
+  </si>
+  <si>
+    <t>http://twitter.com/lhans88/statuses/467763086074466304</t>
+  </si>
+  <si>
+    <t>http://twitter.com/kamkam58/statuses/467848420548681728</t>
+  </si>
+  <si>
+    <t>http://twitter.com/dameonrose/statuses/467813206564413440</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1066,7 +1138,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1347,15 +1419,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP101"/>
+  <dimension ref="A1:AW101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD101"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1464,7 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
@@ -1482,8 +1557,29 @@
       <c r="AP1" t="s">
         <v>41</v>
       </c>
+      <c r="AQ1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>341</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1598,8 +1694,29 @@
       <c r="AP2" t="s">
         <v>46</v>
       </c>
+      <c r="AQ2">
+        <v>236</v>
+      </c>
+      <c r="AR2">
+        <v>295</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>12779</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1714,8 +1831,29 @@
       <c r="AP3" t="s">
         <v>49</v>
       </c>
+      <c r="AQ3">
+        <v>92</v>
+      </c>
+      <c r="AR3">
+        <v>101</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>7331</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1833,8 +1971,29 @@
       <c r="AP4" t="s">
         <v>46</v>
       </c>
+      <c r="AQ4">
+        <v>185</v>
+      </c>
+      <c r="AR4">
+        <v>172</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>3371</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1952,8 +2111,29 @@
       <c r="AP5" t="s">
         <v>49</v>
       </c>
+      <c r="AQ5">
+        <v>165</v>
+      </c>
+      <c r="AR5">
+        <v>94</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>3175</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2068,8 +2248,29 @@
       <c r="AP6" t="s">
         <v>60</v>
       </c>
+      <c r="AQ6">
+        <v>37</v>
+      </c>
+      <c r="AR6">
+        <v>113</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>188</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2187,8 +2388,29 @@
       <c r="AP7" t="s">
         <v>46</v>
       </c>
+      <c r="AQ7">
+        <v>284</v>
+      </c>
+      <c r="AR7">
+        <v>1211</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>166</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2309,8 +2531,29 @@
       <c r="AP8" t="s">
         <v>46</v>
       </c>
+      <c r="AQ8">
+        <v>181</v>
+      </c>
+      <c r="AR8">
+        <v>515</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>343</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>366</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2431,8 +2674,29 @@
       <c r="AP9" t="s">
         <v>60</v>
       </c>
+      <c r="AQ9">
+        <v>253</v>
+      </c>
+      <c r="AR9">
+        <v>828</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>344</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
+        <v>9129</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2550,8 +2814,29 @@
       <c r="AP10" t="s">
         <v>46</v>
       </c>
+      <c r="AQ10">
+        <v>4</v>
+      </c>
+      <c r="AR10">
+        <v>18</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -2669,8 +2954,29 @@
       <c r="AP11" t="s">
         <v>46</v>
       </c>
+      <c r="AQ11">
+        <v>419</v>
+      </c>
+      <c r="AR11">
+        <v>532</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>10827</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2785,8 +3091,29 @@
       <c r="AP12" t="s">
         <v>49</v>
       </c>
+      <c r="AQ12">
+        <v>522</v>
+      </c>
+      <c r="AR12">
+        <v>478</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV12">
+        <v>0</v>
+      </c>
+      <c r="AW12">
+        <v>4747</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -2904,8 +3231,29 @@
       <c r="AP13" t="s">
         <v>46</v>
       </c>
+      <c r="AQ13">
+        <v>58</v>
+      </c>
+      <c r="AR13">
+        <v>399</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV13">
+        <v>0</v>
+      </c>
+      <c r="AW13">
+        <v>101</v>
+      </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3023,8 +3371,29 @@
       <c r="AP14" t="s">
         <v>46</v>
       </c>
+      <c r="AQ14">
+        <v>56</v>
+      </c>
+      <c r="AR14">
+        <v>120</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>180</v>
+      </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3142,8 +3511,29 @@
       <c r="AP15" t="s">
         <v>46</v>
       </c>
+      <c r="AQ15">
+        <v>2191</v>
+      </c>
+      <c r="AR15">
+        <v>23</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV15">
+        <v>1</v>
+      </c>
+      <c r="AW15">
+        <v>108</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3264,8 +3654,29 @@
       <c r="AP16" t="s">
         <v>46</v>
       </c>
+      <c r="AQ16">
+        <v>110</v>
+      </c>
+      <c r="AR16">
+        <v>697</v>
+      </c>
+      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>345</v>
+      </c>
+      <c r="AV16">
+        <v>0</v>
+      </c>
+      <c r="AW16">
+        <v>2217</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3380,8 +3791,29 @@
       <c r="AP17" t="s">
         <v>49</v>
       </c>
+      <c r="AQ17">
+        <v>165</v>
+      </c>
+      <c r="AR17">
+        <v>302</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV17">
+        <v>0</v>
+      </c>
+      <c r="AW17">
+        <v>9214</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -3499,8 +3931,29 @@
       <c r="AP18" t="s">
         <v>46</v>
       </c>
+      <c r="AQ18">
+        <v>2191</v>
+      </c>
+      <c r="AR18">
+        <v>23</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV18">
+        <v>1</v>
+      </c>
+      <c r="AW18">
+        <v>108</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -3618,8 +4071,29 @@
       <c r="AP19" t="s">
         <v>46</v>
       </c>
+      <c r="AQ19">
+        <v>195</v>
+      </c>
+      <c r="AR19">
+        <v>596</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV19">
+        <v>0</v>
+      </c>
+      <c r="AW19">
+        <v>3846</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -3740,8 +4214,29 @@
       <c r="AP20" t="s">
         <v>46</v>
       </c>
+      <c r="AQ20">
+        <v>1292</v>
+      </c>
+      <c r="AR20">
+        <v>697</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>346</v>
+      </c>
+      <c r="AV20">
+        <v>0</v>
+      </c>
+      <c r="AW20">
+        <v>8339</v>
+      </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -3859,8 +4354,29 @@
       <c r="AP21" t="s">
         <v>46</v>
       </c>
+      <c r="AQ21">
+        <v>113</v>
+      </c>
+      <c r="AR21">
+        <v>310</v>
+      </c>
+      <c r="AS21">
+        <v>1</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV21">
+        <v>0</v>
+      </c>
+      <c r="AW21">
+        <v>408</v>
+      </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -3975,8 +4491,29 @@
       <c r="AP22" t="s">
         <v>49</v>
       </c>
+      <c r="AQ22">
+        <v>277</v>
+      </c>
+      <c r="AR22">
+        <v>297</v>
+      </c>
+      <c r="AS22">
+        <v>0</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV22">
+        <v>1</v>
+      </c>
+      <c r="AW22">
+        <v>4048</v>
+      </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -4097,8 +4634,29 @@
       <c r="AP23" t="s">
         <v>46</v>
       </c>
+      <c r="AQ23">
+        <v>9</v>
+      </c>
+      <c r="AR23">
+        <v>90</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV23">
+        <v>0</v>
+      </c>
+      <c r="AW23">
+        <v>524</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -4216,8 +4774,29 @@
       <c r="AP24" t="s">
         <v>46</v>
       </c>
+      <c r="AQ24">
+        <v>2191</v>
+      </c>
+      <c r="AR24">
+        <v>23</v>
+      </c>
+      <c r="AS24">
+        <v>0</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV24">
+        <v>1</v>
+      </c>
+      <c r="AW24">
+        <v>108</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -4338,8 +4917,29 @@
       <c r="AP25" t="s">
         <v>46</v>
       </c>
+      <c r="AQ25">
+        <v>181</v>
+      </c>
+      <c r="AR25">
+        <v>515</v>
+      </c>
+      <c r="AS25">
+        <v>0</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>347</v>
+      </c>
+      <c r="AV25">
+        <v>0</v>
+      </c>
+      <c r="AW25">
+        <v>366</v>
+      </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -4460,8 +5060,29 @@
       <c r="AP26" t="s">
         <v>46</v>
       </c>
+      <c r="AQ26">
+        <v>165</v>
+      </c>
+      <c r="AR26">
+        <v>187</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>343</v>
+      </c>
+      <c r="AV26">
+        <v>0</v>
+      </c>
+      <c r="AW26">
+        <v>725</v>
+      </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -4582,8 +5203,29 @@
       <c r="AP27" t="s">
         <v>46</v>
       </c>
+      <c r="AQ27">
+        <v>1623</v>
+      </c>
+      <c r="AR27">
+        <v>573</v>
+      </c>
+      <c r="AS27">
+        <v>0</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU27" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV27">
+        <v>2</v>
+      </c>
+      <c r="AW27">
+        <v>30300</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -4701,8 +5343,29 @@
       <c r="AP28" t="s">
         <v>46</v>
       </c>
+      <c r="AQ28">
+        <v>2191</v>
+      </c>
+      <c r="AR28">
+        <v>23</v>
+      </c>
+      <c r="AS28">
+        <v>1</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV28">
+        <v>4</v>
+      </c>
+      <c r="AW28">
+        <v>108</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -4823,8 +5486,29 @@
       <c r="AP29" t="s">
         <v>46</v>
       </c>
+      <c r="AQ29">
+        <v>349</v>
+      </c>
+      <c r="AR29">
+        <v>474</v>
+      </c>
+      <c r="AS29">
+        <v>0</v>
+      </c>
+      <c r="AT29" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>348</v>
+      </c>
+      <c r="AV29">
+        <v>0</v>
+      </c>
+      <c r="AW29">
+        <v>582</v>
+      </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -4945,8 +5629,29 @@
       <c r="AP30" t="s">
         <v>46</v>
       </c>
+      <c r="AQ30">
+        <v>1292</v>
+      </c>
+      <c r="AR30">
+        <v>697</v>
+      </c>
+      <c r="AS30">
+        <v>0</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV30">
+        <v>0</v>
+      </c>
+      <c r="AW30">
+        <v>8339</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -5067,8 +5772,29 @@
       <c r="AP31" t="s">
         <v>46</v>
       </c>
+      <c r="AQ31">
+        <v>394</v>
+      </c>
+      <c r="AR31">
+        <v>198</v>
+      </c>
+      <c r="AS31">
+        <v>0</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU31" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV31">
+        <v>0</v>
+      </c>
+      <c r="AW31">
+        <v>13797</v>
+      </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -5189,8 +5915,29 @@
       <c r="AP32" t="s">
         <v>46</v>
       </c>
+      <c r="AQ32">
+        <v>181</v>
+      </c>
+      <c r="AR32">
+        <v>515</v>
+      </c>
+      <c r="AS32">
+        <v>0</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU32" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV32">
+        <v>0</v>
+      </c>
+      <c r="AW32">
+        <v>366</v>
+      </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -5311,8 +6058,29 @@
       <c r="AP33" t="s">
         <v>46</v>
       </c>
+      <c r="AQ33">
+        <v>44</v>
+      </c>
+      <c r="AR33">
+        <v>82</v>
+      </c>
+      <c r="AS33">
+        <v>0</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV33">
+        <v>0</v>
+      </c>
+      <c r="AW33">
+        <v>3782</v>
+      </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -5430,8 +6198,29 @@
       <c r="AP34" t="s">
         <v>46</v>
       </c>
+      <c r="AQ34">
+        <v>227</v>
+      </c>
+      <c r="AR34">
+        <v>99</v>
+      </c>
+      <c r="AS34">
+        <v>0</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV34">
+        <v>0</v>
+      </c>
+      <c r="AW34">
+        <v>11102</v>
+      </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -5549,8 +6338,29 @@
       <c r="AP35" t="s">
         <v>49</v>
       </c>
+      <c r="AQ35">
+        <v>124</v>
+      </c>
+      <c r="AR35">
+        <v>127</v>
+      </c>
+      <c r="AS35">
+        <v>0</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU35" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV35">
+        <v>1</v>
+      </c>
+      <c r="AW35">
+        <v>889</v>
+      </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -5665,8 +6475,29 @@
       <c r="AP36" t="s">
         <v>49</v>
       </c>
+      <c r="AQ36">
+        <v>238</v>
+      </c>
+      <c r="AR36">
+        <v>178</v>
+      </c>
+      <c r="AS36">
+        <v>0</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU36" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV36">
+        <v>0</v>
+      </c>
+      <c r="AW36">
+        <v>22216</v>
+      </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -5781,8 +6612,29 @@
       <c r="AP37" t="s">
         <v>46</v>
       </c>
+      <c r="AQ37">
+        <v>143</v>
+      </c>
+      <c r="AR37">
+        <v>122</v>
+      </c>
+      <c r="AS37">
+        <v>0</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU37" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV37">
+        <v>0</v>
+      </c>
+      <c r="AW37">
+        <v>8954</v>
+      </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -5900,8 +6752,29 @@
       <c r="AP38" t="s">
         <v>46</v>
       </c>
+      <c r="AQ38">
+        <v>19</v>
+      </c>
+      <c r="AR38">
+        <v>39</v>
+      </c>
+      <c r="AS38">
+        <v>0</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU38" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV38">
+        <v>1</v>
+      </c>
+      <c r="AW38">
+        <v>103</v>
+      </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -6022,8 +6895,29 @@
       <c r="AP39" t="s">
         <v>46</v>
       </c>
+      <c r="AQ39">
+        <v>25</v>
+      </c>
+      <c r="AR39">
+        <v>97</v>
+      </c>
+      <c r="AS39">
+        <v>0</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU39" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV39">
+        <v>0</v>
+      </c>
+      <c r="AW39">
+        <v>45</v>
+      </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -6144,8 +7038,29 @@
       <c r="AP40" t="s">
         <v>46</v>
       </c>
+      <c r="AQ40">
+        <v>764</v>
+      </c>
+      <c r="AR40">
+        <v>282</v>
+      </c>
+      <c r="AS40">
+        <v>0</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU40" t="s">
+        <v>348</v>
+      </c>
+      <c r="AV40">
+        <v>0</v>
+      </c>
+      <c r="AW40">
+        <v>4576</v>
+      </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -6263,8 +7178,29 @@
       <c r="AP41" t="s">
         <v>46</v>
       </c>
+      <c r="AQ41">
+        <v>2191</v>
+      </c>
+      <c r="AR41">
+        <v>23</v>
+      </c>
+      <c r="AS41">
+        <v>7</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU41" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV41">
+        <v>14</v>
+      </c>
+      <c r="AW41">
+        <v>108</v>
+      </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -6385,8 +7321,29 @@
       <c r="AP42" t="s">
         <v>46</v>
       </c>
+      <c r="AQ42">
+        <v>181</v>
+      </c>
+      <c r="AR42">
+        <v>515</v>
+      </c>
+      <c r="AS42">
+        <v>0</v>
+      </c>
+      <c r="AT42" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU42" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV42">
+        <v>0</v>
+      </c>
+      <c r="AW42">
+        <v>366</v>
+      </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -6507,8 +7464,29 @@
       <c r="AP43" t="s">
         <v>46</v>
       </c>
+      <c r="AQ43">
+        <v>148</v>
+      </c>
+      <c r="AR43">
+        <v>72</v>
+      </c>
+      <c r="AS43">
+        <v>0</v>
+      </c>
+      <c r="AT43" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV43">
+        <v>0</v>
+      </c>
+      <c r="AW43">
+        <v>2791</v>
+      </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -6629,8 +7607,29 @@
       <c r="AP44" t="s">
         <v>46</v>
       </c>
+      <c r="AQ44">
+        <v>64</v>
+      </c>
+      <c r="AR44">
+        <v>142</v>
+      </c>
+      <c r="AS44">
+        <v>0</v>
+      </c>
+      <c r="AT44" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU44" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV44">
+        <v>0</v>
+      </c>
+      <c r="AW44">
+        <v>87</v>
+      </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -6751,8 +7750,29 @@
       <c r="AP45" t="s">
         <v>46</v>
       </c>
+      <c r="AQ45">
+        <v>186</v>
+      </c>
+      <c r="AR45">
+        <v>113</v>
+      </c>
+      <c r="AS45">
+        <v>0</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU45" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV45">
+        <v>0</v>
+      </c>
+      <c r="AW45">
+        <v>1004</v>
+      </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -6870,8 +7890,29 @@
       <c r="AP46" t="s">
         <v>46</v>
       </c>
+      <c r="AQ46">
+        <v>165</v>
+      </c>
+      <c r="AR46">
+        <v>187</v>
+      </c>
+      <c r="AS46">
+        <v>0</v>
+      </c>
+      <c r="AT46" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU46" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV46">
+        <v>2</v>
+      </c>
+      <c r="AW46">
+        <v>725</v>
+      </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -6992,8 +8033,29 @@
       <c r="AP47" t="s">
         <v>46</v>
       </c>
+      <c r="AQ47">
+        <v>118</v>
+      </c>
+      <c r="AR47">
+        <v>386</v>
+      </c>
+      <c r="AS47">
+        <v>0</v>
+      </c>
+      <c r="AT47" t="s">
+        <v>351</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV47">
+        <v>0</v>
+      </c>
+      <c r="AW47">
+        <v>1370</v>
+      </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -7114,8 +8176,29 @@
       <c r="AP48" t="s">
         <v>46</v>
       </c>
+      <c r="AQ48">
+        <v>512</v>
+      </c>
+      <c r="AR48">
+        <v>360</v>
+      </c>
+      <c r="AS48">
+        <v>0</v>
+      </c>
+      <c r="AT48" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU48" t="s">
+        <v>352</v>
+      </c>
+      <c r="AV48">
+        <v>0</v>
+      </c>
+      <c r="AW48">
+        <v>8691</v>
+      </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -7236,8 +8319,29 @@
       <c r="AP49" t="s">
         <v>46</v>
       </c>
+      <c r="AQ49">
+        <v>19</v>
+      </c>
+      <c r="AR49">
+        <v>55</v>
+      </c>
+      <c r="AS49">
+        <v>0</v>
+      </c>
+      <c r="AT49" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU49" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV49">
+        <v>0</v>
+      </c>
+      <c r="AW49">
+        <v>33</v>
+      </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -7358,8 +8462,29 @@
       <c r="AP50" t="s">
         <v>46</v>
       </c>
+      <c r="AQ50">
+        <v>946</v>
+      </c>
+      <c r="AR50">
+        <v>219</v>
+      </c>
+      <c r="AS50">
+        <v>0</v>
+      </c>
+      <c r="AT50" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU50" t="s">
+        <v>352</v>
+      </c>
+      <c r="AV50">
+        <v>0</v>
+      </c>
+      <c r="AW50">
+        <v>3634</v>
+      </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -7480,8 +8605,29 @@
       <c r="AP51" t="s">
         <v>46</v>
       </c>
+      <c r="AQ51">
+        <v>185</v>
+      </c>
+      <c r="AR51">
+        <v>219</v>
+      </c>
+      <c r="AS51">
+        <v>0</v>
+      </c>
+      <c r="AT51" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU51" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV51">
+        <v>0</v>
+      </c>
+      <c r="AW51">
+        <v>4805</v>
+      </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -7602,8 +8748,29 @@
       <c r="AP52" t="s">
         <v>46</v>
       </c>
+      <c r="AQ52">
+        <v>171</v>
+      </c>
+      <c r="AR52">
+        <v>296</v>
+      </c>
+      <c r="AS52">
+        <v>0</v>
+      </c>
+      <c r="AT52" t="s">
+        <v>353</v>
+      </c>
+      <c r="AU52" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV52">
+        <v>0</v>
+      </c>
+      <c r="AW52">
+        <v>1253</v>
+      </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -7721,8 +8888,29 @@
       <c r="AP53" t="s">
         <v>46</v>
       </c>
+      <c r="AQ53">
+        <v>121</v>
+      </c>
+      <c r="AR53">
+        <v>189</v>
+      </c>
+      <c r="AS53">
+        <v>0</v>
+      </c>
+      <c r="AT53" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU53" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV53">
+        <v>0</v>
+      </c>
+      <c r="AW53">
+        <v>650</v>
+      </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -7840,8 +9028,29 @@
       <c r="AP54" t="s">
         <v>49</v>
       </c>
+      <c r="AQ54">
+        <v>139</v>
+      </c>
+      <c r="AR54">
+        <v>90</v>
+      </c>
+      <c r="AS54">
+        <v>0</v>
+      </c>
+      <c r="AT54" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU54" t="s">
+        <v>354</v>
+      </c>
+      <c r="AV54">
+        <v>0</v>
+      </c>
+      <c r="AW54">
+        <v>481</v>
+      </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -7962,8 +9171,29 @@
       <c r="AP55" t="s">
         <v>46</v>
       </c>
+      <c r="AQ55">
+        <v>51</v>
+      </c>
+      <c r="AR55">
+        <v>106</v>
+      </c>
+      <c r="AS55">
+        <v>0</v>
+      </c>
+      <c r="AT55" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU55" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV55">
+        <v>0</v>
+      </c>
+      <c r="AW55">
+        <v>4924</v>
+      </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
@@ -8081,8 +9311,29 @@
       <c r="AP56" t="s">
         <v>46</v>
       </c>
+      <c r="AQ56">
+        <v>258</v>
+      </c>
+      <c r="AR56">
+        <v>272</v>
+      </c>
+      <c r="AS56">
+        <v>0</v>
+      </c>
+      <c r="AT56" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU56" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV56">
+        <v>0</v>
+      </c>
+      <c r="AW56">
+        <v>1809</v>
+      </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -8200,8 +9451,29 @@
       <c r="AP57" t="s">
         <v>46</v>
       </c>
+      <c r="AQ57">
+        <v>119</v>
+      </c>
+      <c r="AR57">
+        <v>161</v>
+      </c>
+      <c r="AS57">
+        <v>0</v>
+      </c>
+      <c r="AT57" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU57" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV57">
+        <v>0</v>
+      </c>
+      <c r="AW57">
+        <v>631</v>
+      </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0</v>
       </c>
@@ -8316,8 +9588,29 @@
       <c r="AP58" t="s">
         <v>46</v>
       </c>
+      <c r="AQ58">
+        <v>45</v>
+      </c>
+      <c r="AR58">
+        <v>103</v>
+      </c>
+      <c r="AS58">
+        <v>0</v>
+      </c>
+      <c r="AT58" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU58" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV58">
+        <v>0</v>
+      </c>
+      <c r="AW58">
+        <v>399</v>
+      </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -8435,8 +9728,29 @@
       <c r="AP59" t="s">
         <v>46</v>
       </c>
+      <c r="AQ59">
+        <v>34</v>
+      </c>
+      <c r="AR59">
+        <v>32</v>
+      </c>
+      <c r="AS59">
+        <v>0</v>
+      </c>
+      <c r="AT59" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU59" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV59">
+        <v>0</v>
+      </c>
+      <c r="AW59">
+        <v>64</v>
+      </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0</v>
       </c>
@@ -8551,8 +9865,29 @@
       <c r="AP60" t="s">
         <v>46</v>
       </c>
+      <c r="AQ60">
+        <v>488</v>
+      </c>
+      <c r="AR60">
+        <v>470</v>
+      </c>
+      <c r="AS60">
+        <v>0</v>
+      </c>
+      <c r="AT60" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU60" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV60">
+        <v>0</v>
+      </c>
+      <c r="AW60">
+        <v>14700</v>
+      </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -8670,8 +10005,29 @@
       <c r="AP61" t="s">
         <v>46</v>
       </c>
+      <c r="AQ61">
+        <v>261</v>
+      </c>
+      <c r="AR61">
+        <v>495</v>
+      </c>
+      <c r="AS61">
+        <v>0</v>
+      </c>
+      <c r="AT61" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU61" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV61">
+        <v>0</v>
+      </c>
+      <c r="AW61">
+        <v>31588</v>
+      </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -8789,8 +10145,29 @@
       <c r="AP62" t="s">
         <v>46</v>
       </c>
+      <c r="AQ62">
+        <v>177</v>
+      </c>
+      <c r="AR62">
+        <v>144</v>
+      </c>
+      <c r="AS62">
+        <v>0</v>
+      </c>
+      <c r="AT62" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU62" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV62">
+        <v>0</v>
+      </c>
+      <c r="AW62">
+        <v>6525</v>
+      </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -8908,8 +10285,29 @@
       <c r="AP63" t="s">
         <v>46</v>
       </c>
+      <c r="AQ63">
+        <v>78</v>
+      </c>
+      <c r="AR63">
+        <v>150</v>
+      </c>
+      <c r="AS63">
+        <v>0</v>
+      </c>
+      <c r="AT63" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU63" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV63">
+        <v>0</v>
+      </c>
+      <c r="AW63">
+        <v>488</v>
+      </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -9030,8 +10428,29 @@
       <c r="AP64" t="s">
         <v>46</v>
       </c>
+      <c r="AQ64">
+        <v>7097</v>
+      </c>
+      <c r="AR64">
+        <v>313</v>
+      </c>
+      <c r="AS64">
+        <v>0</v>
+      </c>
+      <c r="AT64" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU64" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV64">
+        <v>0</v>
+      </c>
+      <c r="AW64">
+        <v>35596</v>
+      </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -9149,8 +10568,29 @@
       <c r="AP65" t="s">
         <v>46</v>
       </c>
+      <c r="AQ65">
+        <v>205</v>
+      </c>
+      <c r="AR65">
+        <v>255</v>
+      </c>
+      <c r="AS65">
+        <v>0</v>
+      </c>
+      <c r="AT65" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU65" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV65">
+        <v>0</v>
+      </c>
+      <c r="AW65">
+        <v>4497</v>
+      </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -9268,8 +10708,29 @@
       <c r="AP66" t="s">
         <v>46</v>
       </c>
+      <c r="AQ66">
+        <v>14</v>
+      </c>
+      <c r="AR66">
+        <v>34</v>
+      </c>
+      <c r="AS66">
+        <v>0</v>
+      </c>
+      <c r="AT66" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU66" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV66">
+        <v>0</v>
+      </c>
+      <c r="AW66">
+        <v>43</v>
+      </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -9387,8 +10848,29 @@
       <c r="AP67" t="s">
         <v>46</v>
       </c>
+      <c r="AQ67">
+        <v>387</v>
+      </c>
+      <c r="AR67">
+        <v>529</v>
+      </c>
+      <c r="AS67">
+        <v>1</v>
+      </c>
+      <c r="AT67" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU67" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV67">
+        <v>2</v>
+      </c>
+      <c r="AW67">
+        <v>2498</v>
+      </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -9503,8 +10985,29 @@
       <c r="AP68" t="s">
         <v>46</v>
       </c>
+      <c r="AQ68">
+        <v>599</v>
+      </c>
+      <c r="AR68">
+        <v>444</v>
+      </c>
+      <c r="AS68">
+        <v>0</v>
+      </c>
+      <c r="AT68" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU68" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV68">
+        <v>0</v>
+      </c>
+      <c r="AW68">
+        <v>11796</v>
+      </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -9622,8 +11125,29 @@
       <c r="AP69" t="s">
         <v>49</v>
       </c>
+      <c r="AQ69">
+        <v>10</v>
+      </c>
+      <c r="AR69">
+        <v>54</v>
+      </c>
+      <c r="AS69">
+        <v>0</v>
+      </c>
+      <c r="AT69" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU69" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV69">
+        <v>0</v>
+      </c>
+      <c r="AW69">
+        <v>37</v>
+      </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -9744,8 +11268,29 @@
       <c r="AP70" t="s">
         <v>46</v>
       </c>
+      <c r="AQ70">
+        <v>199</v>
+      </c>
+      <c r="AR70">
+        <v>162</v>
+      </c>
+      <c r="AS70">
+        <v>0</v>
+      </c>
+      <c r="AT70" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU70" t="s">
+        <v>355</v>
+      </c>
+      <c r="AV70">
+        <v>0</v>
+      </c>
+      <c r="AW70">
+        <v>954</v>
+      </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -9866,8 +11411,29 @@
       <c r="AP71" t="s">
         <v>46</v>
       </c>
+      <c r="AQ71">
+        <v>87</v>
+      </c>
+      <c r="AR71">
+        <v>98</v>
+      </c>
+      <c r="AS71">
+        <v>0</v>
+      </c>
+      <c r="AT71" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU71" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV71">
+        <v>0</v>
+      </c>
+      <c r="AW71">
+        <v>1603</v>
+      </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -9985,8 +11551,29 @@
       <c r="AP72" t="s">
         <v>46</v>
       </c>
+      <c r="AQ72">
+        <v>111</v>
+      </c>
+      <c r="AR72">
+        <v>184</v>
+      </c>
+      <c r="AS72">
+        <v>0</v>
+      </c>
+      <c r="AT72" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU72" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV72">
+        <v>0</v>
+      </c>
+      <c r="AW72">
+        <v>1365</v>
+      </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -10104,8 +11691,29 @@
       <c r="AP73" t="s">
         <v>46</v>
       </c>
+      <c r="AQ73">
+        <v>241</v>
+      </c>
+      <c r="AR73">
+        <v>239</v>
+      </c>
+      <c r="AS73">
+        <v>0</v>
+      </c>
+      <c r="AT73" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU73" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV73">
+        <v>0</v>
+      </c>
+      <c r="AW73">
+        <v>6937</v>
+      </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -10223,8 +11831,29 @@
       <c r="AP74" t="s">
         <v>46</v>
       </c>
+      <c r="AQ74">
+        <v>65</v>
+      </c>
+      <c r="AR74">
+        <v>126</v>
+      </c>
+      <c r="AS74">
+        <v>0</v>
+      </c>
+      <c r="AT74" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU74" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV74">
+        <v>0</v>
+      </c>
+      <c r="AW74">
+        <v>1298</v>
+      </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -10339,8 +11968,29 @@
       <c r="AP75" t="s">
         <v>60</v>
       </c>
+      <c r="AQ75">
+        <v>195</v>
+      </c>
+      <c r="AR75">
+        <v>200</v>
+      </c>
+      <c r="AS75">
+        <v>0</v>
+      </c>
+      <c r="AT75" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU75" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV75">
+        <v>0</v>
+      </c>
+      <c r="AW75">
+        <v>16142</v>
+      </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -10458,8 +12108,29 @@
       <c r="AP76" t="s">
         <v>60</v>
       </c>
+      <c r="AQ76">
+        <v>547</v>
+      </c>
+      <c r="AR76">
+        <v>504</v>
+      </c>
+      <c r="AS76">
+        <v>0</v>
+      </c>
+      <c r="AT76" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU76" t="s">
+        <v>356</v>
+      </c>
+      <c r="AV76">
+        <v>0</v>
+      </c>
+      <c r="AW76">
+        <v>34181</v>
+      </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0</v>
       </c>
@@ -10580,8 +12251,29 @@
       <c r="AP77" t="s">
         <v>46</v>
       </c>
+      <c r="AQ77">
+        <v>71</v>
+      </c>
+      <c r="AR77">
+        <v>69</v>
+      </c>
+      <c r="AS77">
+        <v>0</v>
+      </c>
+      <c r="AT77" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU77" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV77">
+        <v>0</v>
+      </c>
+      <c r="AW77">
+        <v>2614</v>
+      </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -10702,8 +12394,29 @@
       <c r="AP78" t="s">
         <v>46</v>
       </c>
+      <c r="AQ78">
+        <v>292</v>
+      </c>
+      <c r="AR78">
+        <v>432</v>
+      </c>
+      <c r="AS78">
+        <v>0</v>
+      </c>
+      <c r="AT78" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU78" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV78">
+        <v>0</v>
+      </c>
+      <c r="AW78">
+        <v>9778</v>
+      </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -10824,8 +12537,29 @@
       <c r="AP79" t="s">
         <v>46</v>
       </c>
+      <c r="AQ79">
+        <v>292</v>
+      </c>
+      <c r="AR79">
+        <v>432</v>
+      </c>
+      <c r="AS79">
+        <v>0</v>
+      </c>
+      <c r="AT79" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU79" t="s">
+        <v>355</v>
+      </c>
+      <c r="AV79">
+        <v>0</v>
+      </c>
+      <c r="AW79">
+        <v>9778</v>
+      </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0</v>
       </c>
@@ -10943,8 +12677,29 @@
       <c r="AP80" t="s">
         <v>46</v>
       </c>
+      <c r="AQ80">
+        <v>261</v>
+      </c>
+      <c r="AR80">
+        <v>256</v>
+      </c>
+      <c r="AS80">
+        <v>0</v>
+      </c>
+      <c r="AT80" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU80" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV80">
+        <v>0</v>
+      </c>
+      <c r="AW80">
+        <v>17388</v>
+      </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -11065,8 +12820,29 @@
       <c r="AP81" t="s">
         <v>46</v>
       </c>
+      <c r="AQ81">
+        <v>292</v>
+      </c>
+      <c r="AR81">
+        <v>432</v>
+      </c>
+      <c r="AS81">
+        <v>0</v>
+      </c>
+      <c r="AT81" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU81" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV81">
+        <v>0</v>
+      </c>
+      <c r="AW81">
+        <v>9778</v>
+      </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -11187,8 +12963,29 @@
       <c r="AP82" t="s">
         <v>46</v>
       </c>
+      <c r="AQ82">
+        <v>852</v>
+      </c>
+      <c r="AR82">
+        <v>827</v>
+      </c>
+      <c r="AS82">
+        <v>0</v>
+      </c>
+      <c r="AT82" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU82" t="s">
+        <v>357</v>
+      </c>
+      <c r="AV82">
+        <v>0</v>
+      </c>
+      <c r="AW82">
+        <v>19766</v>
+      </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -11306,8 +13103,29 @@
       <c r="AP83" t="s">
         <v>46</v>
       </c>
+      <c r="AQ83">
+        <v>6</v>
+      </c>
+      <c r="AR83">
+        <v>89</v>
+      </c>
+      <c r="AS83">
+        <v>0</v>
+      </c>
+      <c r="AT83" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU83" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV83">
+        <v>0</v>
+      </c>
+      <c r="AW83">
+        <v>49</v>
+      </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -11425,8 +13243,29 @@
       <c r="AP84" t="s">
         <v>46</v>
       </c>
+      <c r="AQ84">
+        <v>6</v>
+      </c>
+      <c r="AR84">
+        <v>89</v>
+      </c>
+      <c r="AS84">
+        <v>0</v>
+      </c>
+      <c r="AT84" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU84" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV84">
+        <v>0</v>
+      </c>
+      <c r="AW84">
+        <v>49</v>
+      </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -11544,8 +13383,29 @@
       <c r="AP85" t="s">
         <v>46</v>
       </c>
+      <c r="AQ85">
+        <v>306</v>
+      </c>
+      <c r="AR85">
+        <v>72</v>
+      </c>
+      <c r="AS85">
+        <v>0</v>
+      </c>
+      <c r="AT85" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU85" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV85">
+        <v>0</v>
+      </c>
+      <c r="AW85">
+        <v>1840</v>
+      </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -11663,8 +13523,29 @@
       <c r="AP86" t="s">
         <v>46</v>
       </c>
+      <c r="AQ86">
+        <v>36</v>
+      </c>
+      <c r="AR86">
+        <v>323</v>
+      </c>
+      <c r="AS86">
+        <v>0</v>
+      </c>
+      <c r="AT86" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU86" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV86">
+        <v>0</v>
+      </c>
+      <c r="AW86">
+        <v>392</v>
+      </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -11782,8 +13663,29 @@
       <c r="AP87" t="s">
         <v>46</v>
       </c>
+      <c r="AQ87">
+        <v>1623</v>
+      </c>
+      <c r="AR87">
+        <v>573</v>
+      </c>
+      <c r="AS87">
+        <v>0</v>
+      </c>
+      <c r="AT87" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU87" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV87">
+        <v>0</v>
+      </c>
+      <c r="AW87">
+        <v>30300</v>
+      </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -11904,8 +13806,29 @@
       <c r="AP88" t="s">
         <v>46</v>
       </c>
+      <c r="AQ88">
+        <v>53</v>
+      </c>
+      <c r="AR88">
+        <v>134</v>
+      </c>
+      <c r="AS88">
+        <v>0</v>
+      </c>
+      <c r="AT88" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU88" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV88">
+        <v>0</v>
+      </c>
+      <c r="AW88">
+        <v>644</v>
+      </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -12026,8 +13949,29 @@
       <c r="AP89" t="s">
         <v>46</v>
       </c>
+      <c r="AQ89">
+        <v>46</v>
+      </c>
+      <c r="AR89">
+        <v>56</v>
+      </c>
+      <c r="AS89">
+        <v>0</v>
+      </c>
+      <c r="AT89" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU89" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV89">
+        <v>0</v>
+      </c>
+      <c r="AW89">
+        <v>8470</v>
+      </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -12148,8 +14092,29 @@
       <c r="AP90" t="s">
         <v>49</v>
       </c>
+      <c r="AQ90">
+        <v>9</v>
+      </c>
+      <c r="AR90">
+        <v>69</v>
+      </c>
+      <c r="AS90">
+        <v>0</v>
+      </c>
+      <c r="AT90" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU90" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV90">
+        <v>0</v>
+      </c>
+      <c r="AW90">
+        <v>1697</v>
+      </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -12270,8 +14235,29 @@
       <c r="AP91" t="s">
         <v>49</v>
       </c>
+      <c r="AQ91">
+        <v>9</v>
+      </c>
+      <c r="AR91">
+        <v>69</v>
+      </c>
+      <c r="AS91">
+        <v>0</v>
+      </c>
+      <c r="AT91" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU91" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV91">
+        <v>0</v>
+      </c>
+      <c r="AW91">
+        <v>1697</v>
+      </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -12389,8 +14375,29 @@
       <c r="AP92" t="s">
         <v>46</v>
       </c>
+      <c r="AQ92">
+        <v>655</v>
+      </c>
+      <c r="AR92">
+        <v>955</v>
+      </c>
+      <c r="AS92">
+        <v>0</v>
+      </c>
+      <c r="AT92" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU92" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV92">
+        <v>0</v>
+      </c>
+      <c r="AW92">
+        <v>41548</v>
+      </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -12508,8 +14515,29 @@
       <c r="AP93" t="s">
         <v>46</v>
       </c>
+      <c r="AQ93">
+        <v>235</v>
+      </c>
+      <c r="AR93">
+        <v>172</v>
+      </c>
+      <c r="AS93">
+        <v>0</v>
+      </c>
+      <c r="AT93" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU93" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV93">
+        <v>0</v>
+      </c>
+      <c r="AW93">
+        <v>5932</v>
+      </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -12627,8 +14655,29 @@
       <c r="AP94" t="s">
         <v>46</v>
       </c>
+      <c r="AQ94">
+        <v>235</v>
+      </c>
+      <c r="AR94">
+        <v>172</v>
+      </c>
+      <c r="AS94">
+        <v>0</v>
+      </c>
+      <c r="AT94" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU94" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV94">
+        <v>0</v>
+      </c>
+      <c r="AW94">
+        <v>5932</v>
+      </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -12746,8 +14795,29 @@
       <c r="AP95" t="s">
         <v>46</v>
       </c>
+      <c r="AQ95">
+        <v>228</v>
+      </c>
+      <c r="AR95">
+        <v>194</v>
+      </c>
+      <c r="AS95">
+        <v>0</v>
+      </c>
+      <c r="AT95" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU95" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV95">
+        <v>0</v>
+      </c>
+      <c r="AW95">
+        <v>8751</v>
+      </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -12862,8 +14932,29 @@
       <c r="AP96" t="s">
         <v>46</v>
       </c>
+      <c r="AQ96">
+        <v>28</v>
+      </c>
+      <c r="AR96">
+        <v>97</v>
+      </c>
+      <c r="AS96">
+        <v>0</v>
+      </c>
+      <c r="AT96" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU96" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV96">
+        <v>0</v>
+      </c>
+      <c r="AW96">
+        <v>7</v>
+      </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -12981,8 +15072,29 @@
       <c r="AP97" t="s">
         <v>46</v>
       </c>
+      <c r="AQ97">
+        <v>177</v>
+      </c>
+      <c r="AR97">
+        <v>156</v>
+      </c>
+      <c r="AS97">
+        <v>0</v>
+      </c>
+      <c r="AT97" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU97" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV97">
+        <v>0</v>
+      </c>
+      <c r="AW97">
+        <v>1944</v>
+      </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -13097,8 +15209,29 @@
       <c r="AP98" t="s">
         <v>49</v>
       </c>
+      <c r="AQ98">
+        <v>547</v>
+      </c>
+      <c r="AR98">
+        <v>397</v>
+      </c>
+      <c r="AS98">
+        <v>0</v>
+      </c>
+      <c r="AT98" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU98" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV98">
+        <v>0</v>
+      </c>
+      <c r="AW98">
+        <v>10929</v>
+      </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -13216,8 +15349,29 @@
       <c r="AP99" t="s">
         <v>46</v>
       </c>
+      <c r="AQ99">
+        <v>320</v>
+      </c>
+      <c r="AR99">
+        <v>158</v>
+      </c>
+      <c r="AS99">
+        <v>0</v>
+      </c>
+      <c r="AT99" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU99" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV99">
+        <v>0</v>
+      </c>
+      <c r="AW99">
+        <v>8907</v>
+      </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -13335,8 +15489,29 @@
       <c r="AP100" t="s">
         <v>46</v>
       </c>
+      <c r="AQ100">
+        <v>206</v>
+      </c>
+      <c r="AR100">
+        <v>164</v>
+      </c>
+      <c r="AS100">
+        <v>0</v>
+      </c>
+      <c r="AT100" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU100" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV100">
+        <v>0</v>
+      </c>
+      <c r="AW100">
+        <v>4099</v>
+      </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -13456,9 +15631,31 @@
       </c>
       <c r="AP101" t="s">
         <v>46</v>
+      </c>
+      <c r="AQ101">
+        <v>3922</v>
+      </c>
+      <c r="AR101">
+        <v>2162</v>
+      </c>
+      <c r="AS101">
+        <v>0</v>
+      </c>
+      <c r="AT101" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU101" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV101">
+        <v>1</v>
+      </c>
+      <c r="AW101">
+        <v>3212</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>